<commit_message>
solder station keep improving
solder station keep improving
</commit_message>
<xml_diff>
--- a/DIY_solderStation/arduino_wellerSolderStation_hw_2020_July_v5/Weller_WMRP_and_WMRT_thermocouple_voltage_vs_temperature.xlsx
+++ b/DIY_solderStation/arduino_wellerSolderStation_hw_2020_July_v5/Weller_WMRP_and_WMRT_thermocouple_voltage_vs_temperature.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\GitHubRoot\arduino\DIY_solderStation\arduino_wellerSolderStation_hw_2020_July\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRoot\arduino\DIY_solderStation\arduino_wellerSolderStation_hw_2020_July_v5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11080" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11115" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -714,11 +714,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-906831888"/>
-        <c:axId val="-1354713744"/>
+        <c:axId val="44207440"/>
+        <c:axId val="44222672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-906831888"/>
+        <c:axId val="44207440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -805,12 +805,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1354713744"/>
+        <c:crossAx val="44222672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1354713744"/>
+        <c:axId val="44222672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -897,7 +897,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-906831888"/>
+        <c:crossAx val="44207440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1231,23 +1231,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.7" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.64453125"/>
-    <col min="2" max="2" width="12.52734375"/>
-    <col min="3" max="3" width="16.05859375"/>
-    <col min="4" max="4" width="8.5859375"/>
-    <col min="5" max="5" width="10.52734375" customWidth="1"/>
-    <col min="6" max="6" width="20.234375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="29.1171875" style="16" customWidth="1"/>
-    <col min="8" max="1025" width="8.5859375"/>
+    <col min="1" max="1" width="15.6640625"/>
+    <col min="2" max="2" width="12.53125"/>
+    <col min="3" max="3" width="16.06640625"/>
+    <col min="4" max="4" width="8.59765625"/>
+    <col min="5" max="5" width="10.53125" customWidth="1"/>
+    <col min="6" max="6" width="20.19921875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="29.1328125" style="16" customWidth="1"/>
+    <col min="8" max="1025" width="8.59765625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1262,48 +1262,48 @@
         <v>15</v>
       </c>
       <c r="H1">
-        <v>4.9630000000000001</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+        <v>4.9550000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="6">
         <v>0</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="6">
         <v>20</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>30</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>40</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="6">
         <v>50</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="6">
         <v>60</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="6">
         <v>70</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>80</v>
       </c>
@@ -1542,10 +1542,10 @@
       </c>
       <c r="G20" s="16">
         <f t="shared" si="3"/>
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>90</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>100</v>
       </c>
@@ -1592,10 +1592,10 @@
       </c>
       <c r="G22" s="16">
         <f t="shared" si="3"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>110</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="11">
         <v>120</v>
       </c>
@@ -1642,10 +1642,10 @@
       </c>
       <c r="G24" s="16">
         <f t="shared" si="3"/>
-        <v>183</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.5">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="6">
         <v>130</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>140</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>150</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>160</v>
       </c>
@@ -1742,10 +1742,10 @@
       </c>
       <c r="G28" s="16">
         <f t="shared" si="3"/>
-        <v>251</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>170</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>180</v>
       </c>
@@ -1792,10 +1792,10 @@
       </c>
       <c r="G30" s="16">
         <f t="shared" si="3"/>
-        <v>286</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.5">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A31" s="6">
         <v>190</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>200</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>210</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>220</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>230</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A36" s="6">
         <v>240</v>
       </c>
@@ -1942,10 +1942,10 @@
       </c>
       <c r="G36" s="16">
         <f t="shared" si="3"/>
-        <v>394</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.5">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>250</v>
       </c>
@@ -1967,10 +1967,10 @@
       </c>
       <c r="G37" s="16">
         <f t="shared" si="3"/>
-        <v>412</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.5">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>260</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A39" s="6">
         <v>270</v>
       </c>
@@ -2017,10 +2017,10 @@
       </c>
       <c r="G39" s="16">
         <f t="shared" si="3"/>
-        <v>449</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.5">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>280</v>
       </c>
@@ -2042,10 +2042,10 @@
       </c>
       <c r="G40" s="16">
         <f t="shared" si="3"/>
-        <v>467</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.5">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A41" s="6">
         <v>290</v>
       </c>
@@ -2067,10 +2067,10 @@
       </c>
       <c r="G41" s="16">
         <f t="shared" si="3"/>
-        <v>486</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.5">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A42" s="6">
         <v>300</v>
       </c>
@@ -2092,10 +2092,10 @@
       </c>
       <c r="G42" s="16">
         <f t="shared" si="3"/>
-        <v>504</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.5">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>310</v>
       </c>
@@ -2117,10 +2117,10 @@
       </c>
       <c r="G43" s="16">
         <f t="shared" si="3"/>
-        <v>523</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.5">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A44" s="6">
         <v>320</v>
       </c>
@@ -2142,10 +2142,10 @@
       </c>
       <c r="G44" s="16">
         <f t="shared" si="3"/>
-        <v>541</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.5">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>330</v>
       </c>
@@ -2167,10 +2167,10 @@
       </c>
       <c r="G45" s="16">
         <f t="shared" si="3"/>
-        <v>560</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.5">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>340</v>
       </c>
@@ -2192,10 +2192,10 @@
       </c>
       <c r="G46" s="16">
         <f t="shared" si="3"/>
-        <v>578</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.5">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A47" s="6">
         <v>350</v>
       </c>
@@ -2217,10 +2217,10 @@
       </c>
       <c r="G47" s="16">
         <f t="shared" si="3"/>
-        <v>597</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.5">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>360</v>
       </c>
@@ -2242,10 +2242,10 @@
       </c>
       <c r="G48" s="16">
         <f t="shared" si="3"/>
-        <v>615</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.5">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>370</v>
       </c>
@@ -2267,10 +2267,10 @@
       </c>
       <c r="G49" s="16">
         <f t="shared" si="3"/>
-        <v>634</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.5">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>380</v>
       </c>
@@ -2292,10 +2292,10 @@
       </c>
       <c r="G50" s="16">
         <f t="shared" si="3"/>
-        <v>652</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.5">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>390</v>
       </c>
@@ -2317,10 +2317,10 @@
       </c>
       <c r="G51" s="16">
         <f t="shared" si="3"/>
-        <v>670</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.5">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A52" s="6">
         <v>400</v>
       </c>
@@ -2342,10 +2342,10 @@
       </c>
       <c r="G52" s="16">
         <f t="shared" si="3"/>
-        <v>689</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.5">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>410</v>
       </c>
@@ -2367,10 +2367,10 @@
       </c>
       <c r="G53" s="16">
         <f t="shared" si="3"/>
-        <v>707</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.5">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>420</v>
       </c>
@@ -2392,10 +2392,10 @@
       </c>
       <c r="G54" s="16">
         <f t="shared" si="3"/>
-        <v>725</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.5">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>430</v>
       </c>
@@ -2417,10 +2417,10 @@
       </c>
       <c r="G55" s="16">
         <f t="shared" si="3"/>
-        <v>743</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.5">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>440</v>
       </c>
@@ -2442,10 +2442,10 @@
       </c>
       <c r="G56" s="16">
         <f t="shared" si="3"/>
-        <v>761</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.5">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>450</v>
       </c>
@@ -2467,10 +2467,10 @@
       </c>
       <c r="G57" s="16">
         <f t="shared" si="3"/>
-        <v>778</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.5">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A58" s="6">
         <v>460</v>
       </c>
@@ -2492,10 +2492,10 @@
       </c>
       <c r="G58" s="16">
         <f t="shared" si="3"/>
-        <v>796</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.5">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>470</v>
       </c>
@@ -2517,10 +2517,10 @@
       </c>
       <c r="G59" s="16">
         <f t="shared" si="3"/>
-        <v>813</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.5">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>480</v>
       </c>
@@ -2542,10 +2542,10 @@
       </c>
       <c r="G60" s="16">
         <f t="shared" si="3"/>
-        <v>831</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.5">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>490</v>
       </c>
@@ -2567,10 +2567,10 @@
       </c>
       <c r="G61" s="16">
         <f t="shared" si="3"/>
-        <v>848</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.5">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A62" s="6">
         <v>500</v>
       </c>
@@ -2592,7 +2592,7 @@
       </c>
       <c r="G62" s="16">
         <f t="shared" si="3"/>
-        <v>865</v>
+        <v>866</v>
       </c>
     </row>
   </sheetData>

</xml_diff>